<commit_message>
Handles manual import audit Corrected template XLSX file
</commit_message>
<xml_diff>
--- a/app/frontend/templates/XL Bully Import Blank Template.xlsx
+++ b/app/frontend/templates/XL Bully Import Blank Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Projects/DangerousDogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Projects/DangerousDogs/aphw-ddi-portal/app/frontend/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869E07C8-6F42-1540-BA0C-BEA76B18B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E69111-2F32-5942-B412-86F0A2520A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
-  <si>
-    <t>EmailRef</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -89,36 +86,12 @@
     <t>Insurance Start Date</t>
   </si>
   <si>
-    <t>Payment Ref Number</t>
-  </si>
-  <si>
-    <t>Neutered</t>
-  </si>
-  <si>
-    <t>Microchipped</t>
-  </si>
-  <si>
     <t>MicrochipNumber</t>
   </si>
   <si>
-    <t>Follow up Needed</t>
-  </si>
-  <si>
-    <t>Follow Up Reason</t>
-  </si>
-  <si>
     <t>Index Number</t>
   </si>
   <si>
-    <t>Cert Needed</t>
-  </si>
-  <si>
-    <t>Cert Sent</t>
-  </si>
-  <si>
-    <t>Certificate Issued Date</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -140,15 +113,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>THI168JDE5</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>119 Chaplain Street</t>
   </si>
   <si>
@@ -162,6 +126,9 @@
   </si>
   <si>
     <t>example_owner@hotmail.com</t>
+  </si>
+  <si>
+    <t>Certificate Issued</t>
   </si>
 </sst>
 </file>
@@ -512,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676A383D-A5A8-480D-AD44-97C52A15D314}">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -520,34 +487,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" customWidth="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,366 +563,253 @@
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="I2" s="2">
+        <v>27976</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="K2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="M2" s="2">
+        <v>43597</v>
+      </c>
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="2">
-        <v>27976</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="2">
-        <v>43597</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="2">
+      <c r="P2" s="2">
         <v>45187</v>
       </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2">
+      <c r="Q2">
         <v>125478963245879</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2">
+      <c r="R2">
         <v>100001</v>
       </c>
-      <c r="Y2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA2" s="2">
+      <c r="S2" s="2">
         <v>45247</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J3" s="2"/>
-      <c r="L3" s="3"/>
-      <c r="N3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="AA3" s="2">
-        <v>45250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="E4" s="4"/>
-      <c r="J4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="N4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="AA4" s="2">
-        <v>45251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="N5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="AA5" s="2">
-        <v>45251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="N6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="AA6" s="2">
-        <v>45253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="N7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="AA7" s="2">
-        <v>45253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="N8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="AA8" s="2">
-        <v>45254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="N9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="AA9" s="2"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="N10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="AA10" s="2">
-        <v>45257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="N11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="AA11" s="2">
-        <v>45258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="N12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="AA12" s="2">
-        <v>45259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="N13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="AA13" s="2">
-        <v>45260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="N14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="AA14" s="2">
-        <v>45261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="AA15" s="2"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="N16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="AA16" s="2">
-        <v>45265</v>
-      </c>
-    </row>
-    <row r="17" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="N17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="AA17" s="2">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="18" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="N18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="AA18" s="2">
-        <v>45294</v>
-      </c>
-    </row>
-    <row r="19" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="N19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="AA19" s="2">
-        <v>45295</v>
-      </c>
-    </row>
-    <row r="20" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="N20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="AA20" s="2">
-        <v>45301</v>
-      </c>
-    </row>
-    <row r="21" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="N21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="AA21" s="2">
-        <v>45302</v>
-      </c>
-    </row>
-    <row r="22" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="2"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I14" s="2"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I18" s="2"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I19" s="2"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="7"/>
       <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
+      <c r="S22" s="6"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
-      <c r="AA22" s="6">
-        <v>45275</v>
-      </c>
-      <c r="AB22" s="5"/>
-    </row>
-    <row r="23" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="2"/>
+    </row>
+    <row r="23" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="7"/>
       <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
+      <c r="S23" s="6"/>
       <c r="T23" s="5"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="6">
-        <v>45281</v>
-      </c>
-      <c r="AB23" s="5"/>
-    </row>
-    <row r="24" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="2"/>
+    </row>
+    <row r="24" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I24" s="2"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="7"/>
       <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
+      <c r="S24" s="6"/>
       <c r="T24" s="5"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="5"/>
-    </row>
-    <row r="25" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="2"/>
+    </row>
+    <row r="25" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="7"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
+      <c r="S25" s="6"/>
       <c r="T25" s="5"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="6">
-        <v>45306</v>
-      </c>
-      <c r="AB25" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{E8CE3FDB-C2C1-1D4B-ABAF-8DB394A38594}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{E8CE3FDB-C2C1-1D4B-ABAF-8DB394A38594}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1140,18 +987,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1174,18 +1021,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C98003B0-F3CF-4517-B194-AE61A0FF49B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81E6B11C-751C-4834-A173-ADE3A3D27D98}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C98003B0-F3CF-4517-B194-AE61A0FF49B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Handles manual import audit (#163)
* Handles manual import audit
Corrected template XLSX file

* Patch bump

* Reworked

* Patch bump

---------

Co-authored-by: work <jeremy.barnsley@esynergy.co.uk>
</commit_message>
<xml_diff>
--- a/app/frontend/templates/XL Bully Import Blank Template.xlsx
+++ b/app/frontend/templates/XL Bully Import Blank Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Projects/DangerousDogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Projects/DangerousDogs/aphw-ddi-portal/app/frontend/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869E07C8-6F42-1540-BA0C-BEA76B18B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E69111-2F32-5942-B412-86F0A2520A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
-  <si>
-    <t>EmailRef</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -89,36 +86,12 @@
     <t>Insurance Start Date</t>
   </si>
   <si>
-    <t>Payment Ref Number</t>
-  </si>
-  <si>
-    <t>Neutered</t>
-  </si>
-  <si>
-    <t>Microchipped</t>
-  </si>
-  <si>
     <t>MicrochipNumber</t>
   </si>
   <si>
-    <t>Follow up Needed</t>
-  </si>
-  <si>
-    <t>Follow Up Reason</t>
-  </si>
-  <si>
     <t>Index Number</t>
   </si>
   <si>
-    <t>Cert Needed</t>
-  </si>
-  <si>
-    <t>Cert Sent</t>
-  </si>
-  <si>
-    <t>Certificate Issued Date</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -140,15 +113,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>THI168JDE5</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>119 Chaplain Street</t>
   </si>
   <si>
@@ -162,6 +126,9 @@
   </si>
   <si>
     <t>example_owner@hotmail.com</t>
+  </si>
+  <si>
+    <t>Certificate Issued</t>
   </si>
 </sst>
 </file>
@@ -512,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676A383D-A5A8-480D-AD44-97C52A15D314}">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -520,34 +487,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" customWidth="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,366 +563,253 @@
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="I2" s="2">
+        <v>27976</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="K2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="M2" s="2">
+        <v>43597</v>
+      </c>
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="2">
-        <v>27976</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="2">
-        <v>43597</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="2">
+      <c r="P2" s="2">
         <v>45187</v>
       </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2">
+      <c r="Q2">
         <v>125478963245879</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2">
+      <c r="R2">
         <v>100001</v>
       </c>
-      <c r="Y2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA2" s="2">
+      <c r="S2" s="2">
         <v>45247</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J3" s="2"/>
-      <c r="L3" s="3"/>
-      <c r="N3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="AA3" s="2">
-        <v>45250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="E4" s="4"/>
-      <c r="J4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="N4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="AA4" s="2">
-        <v>45251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="N5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="AA5" s="2">
-        <v>45251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="N6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="AA6" s="2">
-        <v>45253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="N7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="AA7" s="2">
-        <v>45253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="N8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="AA8" s="2">
-        <v>45254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="N9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="AA9" s="2"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="N10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="AA10" s="2">
-        <v>45257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="N11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="AA11" s="2">
-        <v>45258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="N12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="AA12" s="2">
-        <v>45259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="N13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="AA13" s="2">
-        <v>45260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="N14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="AA14" s="2">
-        <v>45261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="AA15" s="2"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="N16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="AA16" s="2">
-        <v>45265</v>
-      </c>
-    </row>
-    <row r="17" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="N17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="AA17" s="2">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="18" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="N18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="AA18" s="2">
-        <v>45294</v>
-      </c>
-    </row>
-    <row r="19" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="N19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="AA19" s="2">
-        <v>45295</v>
-      </c>
-    </row>
-    <row r="20" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="N20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="AA20" s="2">
-        <v>45301</v>
-      </c>
-    </row>
-    <row r="21" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="N21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="AA21" s="2">
-        <v>45302</v>
-      </c>
-    </row>
-    <row r="22" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="2"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I14" s="2"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I18" s="2"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I19" s="2"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="7"/>
       <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
+      <c r="S22" s="6"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
-      <c r="AA22" s="6">
-        <v>45275</v>
-      </c>
-      <c r="AB22" s="5"/>
-    </row>
-    <row r="23" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="2"/>
+    </row>
+    <row r="23" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="7"/>
       <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
+      <c r="S23" s="6"/>
       <c r="T23" s="5"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="6">
-        <v>45281</v>
-      </c>
-      <c r="AB23" s="5"/>
-    </row>
-    <row r="24" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="2"/>
+    </row>
+    <row r="24" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I24" s="2"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="7"/>
       <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
+      <c r="S24" s="6"/>
       <c r="T24" s="5"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="5"/>
-    </row>
-    <row r="25" spans="10:28" x14ac:dyDescent="0.2">
-      <c r="J25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="2"/>
+    </row>
+    <row r="25" spans="9:20" x14ac:dyDescent="0.2">
+      <c r="I25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="7"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
+      <c r="S25" s="6"/>
       <c r="T25" s="5"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="6">
-        <v>45306</v>
-      </c>
-      <c r="AB25" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{E8CE3FDB-C2C1-1D4B-ABAF-8DB394A38594}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{E8CE3FDB-C2C1-1D4B-ABAF-8DB394A38594}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1140,18 +987,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1174,18 +1021,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C98003B0-F3CF-4517-B194-AE61A0FF49B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81E6B11C-751C-4834-A173-ADE3A3D27D98}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C98003B0-F3CF-4517-B194-AE61A0FF49B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>